<commit_message>
Add tubing adapters to BOM
</commit_message>
<xml_diff>
--- a/HMS-Olfactometer-v4-BOM.xlsx
+++ b/HMS-Olfactometer-v4-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ofer/HMS Dropbox/RIC/Projects/Datta - Olfactometer v4/HMS_Olfactometer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C812355-448F-434D-A8CC-CB1F7023F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D755244D-88F3-7442-BB68-16F1D9E4F686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="46080" windowHeight="25420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="106">
   <si>
     <t>Vendor</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t>XXXXX</t>
+  </si>
+  <si>
+    <t>2171-QSPK18-1/4-U-ND</t>
+  </si>
+  <si>
+    <t>1/4" Tubing Adptor for MFCs (10 pack)</t>
+  </si>
+  <si>
+    <t>Helpful if using 1/4" OD Tubing; Otherwise MFCs will work with 6mm OD tubing</t>
   </si>
 </sst>
 </file>
@@ -868,11 +877,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K41"/>
+  <dimension ref="A2:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -881,7 +890,7 @@
     <col min="2" max="2" width="13.875" style="8" customWidth="1"/>
     <col min="3" max="3" width="23.875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="6" max="6" width="25.125" customWidth="1"/>
     <col min="7" max="7" width="3.875" customWidth="1"/>
     <col min="8" max="9" width="10.625" style="9"/>
     <col min="10" max="10" width="3.375" customWidth="1"/>
@@ -976,31 +985,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9">
-        <v>48</v>
-      </c>
-      <c r="H9" s="9">
-        <v>53.07</v>
-      </c>
-      <c r="I9" s="9">
-        <f t="shared" ref="I9:I34" si="0">G9*H9</f>
-        <v>2547.36</v>
-      </c>
-      <c r="K9" t="s">
-        <v>83</v>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>24.3</v>
+      </c>
+      <c r="I8" s="9">
+        <f>G8*H8</f>
+        <v>24.3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1008,26 +1017,26 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="H10" s="9">
-        <v>102.01</v>
+        <v>53.07</v>
       </c>
       <c r="I10" s="9">
-        <f t="shared" si="0"/>
-        <v>612.06000000000006</v>
+        <f t="shared" ref="I10:I35" si="0">G10*H10</f>
+        <v>2547.36</v>
       </c>
       <c r="K10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1035,83 +1044,77 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11" s="9">
+        <v>102.01</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" si="0"/>
+        <v>612.06000000000006</v>
+      </c>
+      <c r="K11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
         <v>85</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>8</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H12" s="9">
         <v>60</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I12" s="9">
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>1</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H14" s="9">
         <v>33</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I14" s="9">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K14" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15" s="9">
-        <v>1.18</v>
-      </c>
-      <c r="I15" s="9">
-        <f t="shared" si="0"/>
-        <v>2.36</v>
-      </c>
-      <c r="K15" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1119,29 +1122,32 @@
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="9">
-        <v>0.15</v>
+        <v>1.18</v>
       </c>
       <c r="I16" s="9">
         <f t="shared" si="0"/>
-        <v>0.15</v>
+        <v>2.36</v>
       </c>
       <c r="K16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1149,26 +1155,29 @@
         <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>58</v>
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="G17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H17" s="9">
-        <v>1.43</v>
+        <v>0.15</v>
       </c>
       <c r="I17" s="9">
         <f t="shared" si="0"/>
-        <v>8.58</v>
+        <v>0.15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1176,23 +1185,26 @@
         <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
       <c r="G18">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1.43</v>
       </c>
       <c r="I18" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K18" t="s">
-        <v>95</v>
+        <v>8.58</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1200,26 +1212,23 @@
         <v>11</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F19" t="s">
-        <v>17</v>
-      </c>
       <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0.61</v>
+        <v>8</v>
       </c>
       <c r="I19" s="9">
         <f t="shared" si="0"/>
-        <v>0.61</v>
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1227,29 +1236,26 @@
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H20" s="9">
-        <v>1.02</v>
+        <v>0.61</v>
       </c>
       <c r="I20" s="9">
         <f t="shared" si="0"/>
-        <v>4.08</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1257,29 +1263,29 @@
         <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="G21">
         <v>4</v>
       </c>
       <c r="H21" s="9">
-        <v>4.6900000000000004</v>
+        <v>1.02</v>
       </c>
       <c r="I21" s="9">
         <f t="shared" si="0"/>
-        <v>18.760000000000002</v>
-      </c>
-      <c r="K21" t="s">
-        <v>96</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1287,26 +1293,29 @@
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H22" s="9">
-        <v>0.93</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="I22" s="9">
         <f t="shared" si="0"/>
-        <v>0.93</v>
+        <v>18.760000000000002</v>
+      </c>
+      <c r="K22" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1314,29 +1323,26 @@
         <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" s="9">
-        <v>0.52</v>
+        <v>0.93</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" si="0"/>
-        <v>0.52</v>
-      </c>
-      <c r="K23" t="s">
-        <v>100</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1344,21 +1350,29 @@
         <v>16</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>99</v>
+      </c>
       <c r="G24">
         <v>1</v>
       </c>
+      <c r="H24" s="9">
+        <v>0.52</v>
+      </c>
       <c r="I24" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.52</v>
+      </c>
+      <c r="K24" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1366,13 +1380,13 @@
         <v>17</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="E25" s="3"/>
       <c r="G25">
@@ -1388,13 +1402,13 @@
         <v>18</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="3"/>
       <c r="G26">
@@ -1410,14 +1424,15 @@
         <v>19</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E27" s="3"/>
       <c r="G27">
         <v>1</v>
       </c>
@@ -1431,16 +1446,16 @@
         <v>20</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I28" s="9">
         <f t="shared" si="0"/>
@@ -1452,32 +1467,20 @@
         <v>21</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29" s="9">
-        <v>3.92</v>
+        <v>5</v>
       </c>
       <c r="I29" s="9">
         <f t="shared" si="0"/>
-        <v>3.92</v>
-      </c>
-      <c r="K29" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1485,84 +1488,84 @@
         <v>22</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" t="s">
-        <v>25</v>
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30" s="9">
-        <v>26.8</v>
+        <v>3.92</v>
       </c>
       <c r="I30" s="9">
         <f t="shared" si="0"/>
-        <v>26.8</v>
+        <v>3.92</v>
+      </c>
+      <c r="K30" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>23</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>11</v>
+        <v>79</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="G31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31" s="9">
-        <v>0.87</v>
+        <v>26.8</v>
       </c>
       <c r="I31" s="9">
         <f t="shared" si="0"/>
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="38" x14ac:dyDescent="0.2">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>24</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="B32" s="4"/>
       <c r="C32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G32">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H32" s="9">
-        <v>2.41</v>
+        <v>0.87</v>
       </c>
       <c r="I32" s="9">
         <f t="shared" si="0"/>
-        <v>16.87</v>
-      </c>
-      <c r="K32" t="s">
-        <v>77</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="38" x14ac:dyDescent="0.2">
@@ -1570,109 +1573,142 @@
         <v>25</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G33">
         <v>7</v>
       </c>
       <c r="H33" s="9">
-        <v>1.54</v>
+        <v>2.41</v>
       </c>
       <c r="I33" s="9">
         <f t="shared" si="0"/>
-        <v>10.780000000000001</v>
+        <v>16.87</v>
       </c>
       <c r="K33" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="38" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>26</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34" s="9">
+        <v>1.54</v>
+      </c>
+      <c r="I34" s="9">
+        <f t="shared" si="0"/>
+        <v>10.780000000000001</v>
+      </c>
+      <c r="K34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>67</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="E35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
         <v>78</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>1</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H35" s="9">
         <v>11.94</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I35" s="9">
         <f t="shared" si="0"/>
         <v>11.94</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>27</v>
-      </c>
-      <c r="C36" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>28</v>
-      </c>
-      <c r="C38" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
         <v>12</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>13</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>94</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <v>6</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H39" s="9">
         <v>0.63</v>
       </c>
-      <c r="I38" s="9">
-        <f t="shared" ref="I38" si="1">G38*H38</f>
+      <c r="I39" s="9">
+        <f t="shared" ref="I39" si="1">G39*H39</f>
         <v>3.7800000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H41" s="2" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H42" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I41" s="2">
-        <f>SUM(I6:I40)</f>
-        <v>4601.2399999999989</v>
+      <c r="I42" s="2">
+        <f>SUM(I6:I41)</f>
+        <v>4625.5399999999981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>